<commit_message>
2nd feature code added
</commit_message>
<xml_diff>
--- a/gg.xlsx
+++ b/gg.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anand\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9147fed4ff88129f/Desktop/auto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39AE491A-19F2-41CB-840B-D7C7DE21764E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_F25DC773A252ABDACC10488F119A7DDC5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7913748-9A5B-45CE-A88D-A69AD37CA616}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{96592F00-52FE-46DA-AE94-42A4FDB16A04}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,19 +25,165 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+  <si>
+    <t>biz.anandvk@gmail.com</t>
+  </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Companies</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
+  <si>
+    <t>soumyamanoria12@gmail.com</t>
+  </si>
+  <si>
+    <t>satish.av@orangewood.co</t>
+  </si>
+  <si>
+    <t>aditya.b@orangewood.co</t>
+  </si>
+  <si>
+    <t>pratiksha.m@greyorange.com</t>
+  </si>
+  <si>
+    <t>preeti.verma@trianz.com</t>
+  </si>
+  <si>
+    <t>shivansh.s@greyorange.com</t>
+  </si>
+  <si>
+    <t>sachin.kamble@ideaforge.co.in</t>
+  </si>
+  <si>
+    <t>her-prishita@flytbase.com</t>
+  </si>
+  <si>
+    <t>pavan.dasari@svayarobotics.com</t>
+  </si>
+  <si>
+    <t>tarun@clutterbot.com</t>
+  </si>
+  <si>
+    <t>deepak.kumbhar@sedemac.com</t>
+  </si>
+  <si>
+    <t>mithila.chavan@sedemac.com</t>
+  </si>
+  <si>
+    <t>yashada.shekdar@unboxrobotics.com</t>
+  </si>
+  <si>
+    <t>sudhakar.n@fanucindia.com</t>
+  </si>
+  <si>
+    <t>srishti.basu@delhivery.com</t>
+  </si>
+  <si>
+    <t>yathursini.ruban@mphasis.com</t>
+  </si>
+  <si>
+    <t>swathi.sushilan@uipath.com</t>
+  </si>
+  <si>
+    <t>radhika.sonar@getpeppermint.co</t>
+  </si>
+  <si>
+    <t>rakesh.kumar@continental-engines.com</t>
+  </si>
+  <si>
+    <t>swati.sinha@aliyancemech.com</t>
+  </si>
+  <si>
+    <t>uchakma@bastiansolutions.com</t>
+  </si>
+  <si>
+    <t>ankita@bastiansolutions.com</t>
+  </si>
+  <si>
+    <t>pragati.bhat@miko.ai</t>
+  </si>
+  <si>
+    <t>sonaldevi.pandey@miko.ai</t>
+  </si>
+  <si>
+    <t>poulomi.bhakta@addverb.com</t>
+  </si>
+  <si>
+    <t>pramod.ghute@in.abb.com</t>
+  </si>
+  <si>
+    <t>supriya.kumari@kuka.com</t>
+  </si>
+  <si>
+    <t>nehaa@gridbots.com</t>
+  </si>
+  <si>
+    <t>athira.raj@simelabs.com</t>
+  </si>
+  <si>
+    <t>gunjan@eternalrobotics.com</t>
+  </si>
+  <si>
+    <t>k.tejaswi@eternalrobotics.com</t>
+  </si>
+  <si>
+    <t>nigel@nebularobotics.com</t>
+  </si>
+  <si>
+    <t>namita.shinde@cybernetik.com</t>
+  </si>
+  <si>
+    <t>srinidhi.mp@dimaag.ai</t>
+  </si>
+  <si>
+    <t>ravinder.kumar@skytechrobotics.in</t>
+  </si>
+  <si>
+    <t>revathi.prabhakara@rapyuta-robotics.com</t>
+  </si>
+  <si>
+    <t>hemanta.pradhan@nxtwave.co.in</t>
+  </si>
+  <si>
+    <t>manila.d.kapoor@medtronic.com</t>
+  </si>
+  <si>
+    <t>anmolas@wipropari.com</t>
+  </si>
+  <si>
+    <t>ravinder.k@orangewood.co</t>
+  </si>
+  <si>
+    <t>gourav.s@greyorange.com</t>
+  </si>
+  <si>
+    <t>yashada.s@unboxrobotics.com</t>
+  </si>
+  <si>
+    <t>Put to be mailed under 'Email' column</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -60,16 +206,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -83,6 +237,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -102,7 +280,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -114,7 +292,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -161,23 +339,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -213,23 +374,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -381,21 +525,251 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEFA1B3-AA07-4EB3-9F7A-9F828F6AF341}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="46.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C60" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AA817CD3-DD4B-460F-9995-A2AD7B8AA770}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>